<commit_message>
OPSK-1185 Test to reproduce error
</commit_message>
<xml_diff>
--- a/test/fixtures/files/strain-sample-data.xlsx
+++ b/test/fixtures/files/strain-sample-data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>some stuff</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>seekstrain</t>
+  </si>
+  <si>
+    <t>optionalstrain</t>
   </si>
   <si>
     <t>Bob Monkhouse</t>
@@ -177,17 +180,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9028340080972"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,10 +201,13 @@
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>29823659</v>
@@ -208,15 +215,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>29823659</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>29823659</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1234</v>
@@ -224,7 +234,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>